<commit_message>
update to navigation and 3.14 and one NZGrapher video
</commit_message>
<xml_diff>
--- a/nzgrapher/left.xlsx
+++ b/nzgrapher/left.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakew\Dropbox\Documents\GitHub\students.mathsnz.com\nzgrapher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakew\GitHub\students.mathsnz.com\nzgrapher\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DE1DE6-2D7F-4DBA-A1BD-60A681C5A58A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="15360" windowHeight="4740"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="15360" windowHeight="4740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>&lt;/a&gt;</t>
   </si>
@@ -122,9 +123,6 @@
     <t>Part 3.4: Paired Experimental Data (Including Arrows Graphs)</t>
   </si>
   <si>
-    <t>Part 3.5: Dotplots and Informal Confidence Intervals</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -155,9 +153,6 @@
     <t>hgi1IQYPBX8</t>
   </si>
   <si>
-    <t>H15YmE99iKI</t>
-  </si>
-  <si>
     <t>AWG11RalTXI</t>
   </si>
   <si>
@@ -167,9 +162,6 @@
     <t>8BGX_LrP0qc</t>
   </si>
   <si>
-    <t>PDyLsvunSpw</t>
-  </si>
-  <si>
     <t>OXvbLmIsk_Y</t>
   </si>
   <si>
@@ -189,12 +181,15 @@
   </si>
   <si>
     <t>aaDQ6GHCtwA</t>
+  </si>
+  <si>
+    <t>mZI-W7w__r0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,20 +503,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" customWidth="1"/>
-    <col min="2" max="2" width="55.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -556,9 +551,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A23" si="0">"&lt;a href='"&amp;H2&amp;".html'"&amp;I2&amp;"&gt;"</f>
+        <f t="shared" ref="A2:A22" si="0">"&lt;a href='"&amp;H2&amp;".html'"&amp;I2&amp;"&gt;"</f>
         <v>&lt;a href='nzgrapher_a.html'&gt;</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -579,7 +574,7 @@
         <v>nzgrapher_a</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_1.html' class='indent'&gt;</v>
@@ -603,7 +598,7 @@
         <v>a_1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H23" si="1">"nzgrapher_"&amp;G3</f>
+        <f t="shared" ref="H3:H22" si="1">"nzgrapher_"&amp;G3</f>
         <v>nzgrapher_a_1</v>
       </c>
       <c r="I3" t="str">
@@ -611,10 +606,10 @@
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_2.html' class='indent'&gt;</v>
@@ -634,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G14" si="2">"a_"&amp;SUBSTITUTE(F4,".","_")</f>
+        <f t="shared" ref="G4:G13" si="2">"a_"&amp;SUBSTITUTE(F4,".","_")</f>
         <v>a_2</v>
       </c>
       <c r="H4" t="str">
@@ -642,14 +637,14 @@
         <v>nzgrapher_a_2</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I21" si="3">" class='indent'"</f>
+        <f t="shared" ref="I4:I20" si="3">" class='indent'"</f>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_3.html' class='indent'&gt;</v>
@@ -661,11 +656,11 @@
         <v>0</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E14" si="4">LEFT(B5,FIND(":",B5)-1)</f>
+        <f t="shared" ref="E5:E13" si="4">LEFT(B5,FIND(":",B5)-1)</f>
         <v>Part 3</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F14" si="5">RIGHT(E5,LEN(E5)-FIND(" ",E5))</f>
+        <f t="shared" ref="F5:F13" si="5">RIGHT(E5,LEN(E5)-FIND(" ",E5))</f>
         <v>3</v>
       </c>
       <c r="G5" t="str">
@@ -681,10 +676,10 @@
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_3_1.html' class='indent'&gt;</v>
@@ -716,10 +711,10 @@
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_3_2.html' class='indent'&gt;</v>
@@ -751,16 +746,16 @@
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_3_3.html' class='indent'&gt;</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -786,10 +781,10 @@
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href='nzgrapher_a_3_4.html' class='indent'&gt;</v>
@@ -825,188 +820,176 @@
         <v>-lLHgGsxCQQ</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_a_3_5.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_a_4.html' class='indent'&gt;</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
-        <v>Part 3.5</v>
+        <v>Part 4</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="5"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>a_3_5</v>
+        <v>a_4</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_a_3_5</v>
+        <v>nzgrapher_a_4</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_a_4.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_a_5.html' class='indent'&gt;</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
-        <v>Part 4</v>
+        <v>Part 5</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="2"/>
-        <v>a_4</v>
+        <v>a_5</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_a_4</v>
+        <v>nzgrapher_a_5</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_a_5.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_a_6.html' class='indent'&gt;</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="4"/>
-        <v>Part 5</v>
+        <v>Part 6</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
-        <v>a_5</v>
+        <v>a_6</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_a_5</v>
+        <v>nzgrapher_a_6</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_a_6.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_a_6_1.html' class='indent'&gt;</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="4"/>
-        <v>Part 6</v>
+        <v>Part 6.1</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>a_6</v>
+        <v>a_6_1</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_a_6</v>
+        <v>nzgrapher_a_6_1</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_a_6_1.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b.html'&gt;</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="str">
-        <f t="shared" si="4"/>
-        <v>Part 6.1</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="5"/>
-        <v>6.1</v>
+      <c r="F14" t="s">
+        <v>32</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v>a_6_1</v>
+        <f t="shared" ref="G14:G22" si="6">SUBSTITUTE(F14,".","_")</f>
+        <v>b</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_a_6_1</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> class='indent'</v>
-      </c>
-      <c r="J14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>nzgrapher_b</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b.html'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_1.html' class='indent'&gt;</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1015,21 +998,31 @@
         <v>33</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" ref="G15:G23" si="6">SUBSTITUTE(F15,".","_")</f>
-        <v>b</v>
+        <f t="shared" si="6"/>
+        <v>b_1</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>nzgrapher_b_1</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> class='indent'</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_1.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_2.html' class='indent'&gt;</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -1039,30 +1032,28 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>b_1</v>
+        <v>b_2</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_1</v>
+        <v>nzgrapher_b_2</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
-      <c r="J16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J16" t="str">
+        <f>"-lLHgGsxCQQ"</f>
+        <v>-lLHgGsxCQQ</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_2.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_3.html' class='indent'&gt;</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -1072,28 +1063,27 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>b_2</v>
+        <v>b_3</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_2</v>
+        <v>nzgrapher_b_3</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
-      <c r="J17" t="str">
-        <f>"-lLHgGsxCQQ"</f>
-        <v>-lLHgGsxCQQ</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_3.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_4.html' class='indent'&gt;</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -1103,27 +1093,30 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>b_3</v>
+        <v>b_4</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_3</v>
+        <v>nzgrapher_b_4</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="K18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_4.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_5.html' class='indent'&gt;</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1133,30 +1126,30 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>b_4</v>
+        <v>b_5</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_4</v>
+        <v>nzgrapher_b_5</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> class='indent'</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_5.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_b_6.html' class='indent'&gt;</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -1166,11 +1159,11 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>b_5</v>
+        <v>b_6</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_5</v>
+        <v>nzgrapher_b_6</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="3"/>
@@ -1183,13 +1176,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_b_6.html' class='indent'&gt;</v>
+        <v>&lt;a href='nzgrapher_c.html'&gt;</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -1199,30 +1192,20 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>b_6</v>
+        <v>c</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_b_6</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> class='indent'</v>
-      </c>
-      <c r="J21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>nzgrapher_c</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_c.html'&gt;</v>
+        <v>&lt;a href='nzgrapher_d.html'&gt;</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1232,37 +1215,14 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>c</v>
+        <v>d</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>nzgrapher_c</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href='nzgrapher_d.html'&gt;</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="6"/>
-        <v>d</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="1"/>
         <v>nzgrapher_d</v>
       </c>
-      <c r="J23" t="s">
-        <v>52</v>
+      <c r="J22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>